<commit_message>
[BRD] Fixed reference designator for header in BoM
</commit_message>
<xml_diff>
--- a/dcsense-board/3.1-ryanoshea-final-miniaturized-version/V3_design_pkg1/bom/bom.xlsx
+++ b/dcsense-board/3.1-ryanoshea-final-miniaturized-version/V3_design_pkg1/bom/bom.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\OneDrive\Princeton\Senior\Thesis\V3\V3_design_pkg0\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04dfa027adf204b4/Princeton/Senior/Thesis/data-center-monitoring/dcsense-board/3.1-ryanoshea-final-miniaturized-version/V3_design_pkg1/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="13335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="13340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="158001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -161,9 +164,6 @@
     <t>TI SENSOR TEMPERATURE SMBUS 8MSOP TMP175</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -180,12 +180,15 @@
   </si>
   <si>
     <t>U1</t>
+  </si>
+  <si>
+    <t>J1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,11 +245,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -528,29 +532,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H6:H7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -576,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -584,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>28</v>
@@ -598,11 +602,11 @@
       <c r="G2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -610,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -628,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -636,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -654,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -662,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -680,7 +684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -688,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
@@ -706,7 +710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -714,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -732,7 +736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -740,7 +744,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>

</xml_diff>